<commit_message>
Fix merge conflicts and update scenario names
</commit_message>
<xml_diff>
--- a/analysis/library/investments/scenario-investments.xlsx
+++ b/analysis/library/investments/scenario-investments.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhemez/Floating-CORAL/CORAL/analysis/library/investments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\West Coast ports\Analysis\Deployment\CORAL\analysis\library\investments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1398256-20C1-144D-9E40-36EBE12D37B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F1B71D-9CFA-487F-A1A3-9DA2AF2A9F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="540" windowWidth="30780" windowHeight="18780" activeTab="1" xr2:uid="{D6119032-A265-B843-9C0C-F79837C83C57}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{D6119032-A265-B843-9C0C-F79837C83C57}"/>
   </bookViews>
   <sheets>
     <sheet name="Port-investments" sheetId="1" r:id="rId1"/>
     <sheet name="schedule" sheetId="7" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -85,40 +84,40 @@
     <t>Stand-in numbers:</t>
   </si>
   <si>
-    <t>Baseline-low</t>
-  </si>
-  <si>
-    <t>Baseline-low-annual</t>
-  </si>
-  <si>
-    <t>Baseline-mid-SC-annual</t>
-  </si>
-  <si>
-    <t>Baseline-mid-SC</t>
-  </si>
-  <si>
-    <t>Baseline-mid-CC-annual</t>
-  </si>
-  <si>
-    <t>Baseline-mid-CC</t>
-  </si>
-  <si>
-    <t>Moderate-low-annual</t>
-  </si>
-  <si>
-    <t>Moderate-low</t>
-  </si>
-  <si>
-    <t>Moderate-mid-SC-annual</t>
-  </si>
-  <si>
-    <t>Moderate-mid-SC</t>
-  </si>
-  <si>
-    <t>Expanded-high-annual</t>
-  </si>
-  <si>
-    <t>Expanded-high</t>
+    <t>Baseline-Low-annual</t>
+  </si>
+  <si>
+    <t>Baseline-Low</t>
+  </si>
+  <si>
+    <t>Baseline-Mid (SC)-annual</t>
+  </si>
+  <si>
+    <t>Baseline-Mid (SC)</t>
+  </si>
+  <si>
+    <t>Baseline-Mid (CC)-annual</t>
+  </si>
+  <si>
+    <t>Baseline-Mid (CC)</t>
+  </si>
+  <si>
+    <t>Moderate-Low-annual</t>
+  </si>
+  <si>
+    <t>Moderate-Low</t>
+  </si>
+  <si>
+    <t>Moderate-Mid (SC)-annual</t>
+  </si>
+  <si>
+    <t>Moderate-Mid (SC)</t>
+  </si>
+  <si>
+    <t>Expanded-High-annual</t>
+  </si>
+  <si>
+    <t>Expanded-High</t>
   </si>
 </sst>
 </file>
@@ -485,7 +484,7 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.5" customWidth="1"/>
@@ -498,7 +497,7 @@
     <col min="9" max="9" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,7 +523,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -553,7 +552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -582,7 +581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -605,7 +604,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -628,7 +627,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -651,7 +650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -674,7 +673,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -697,7 +696,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>13</v>
       </c>
@@ -732,11 +731,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61820F40-12B7-8847-B5DA-61E36DFB9194}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
@@ -752,15 +751,15 @@
     <col min="13" max="13" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>17</v>
@@ -793,7 +792,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2029</v>
       </c>
@@ -834,7 +833,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2030</v>
       </c>
@@ -881,7 +880,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2031</v>
       </c>
@@ -928,7 +927,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2032</v>
       </c>
@@ -975,7 +974,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2033</v>
       </c>
@@ -1022,7 +1021,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2034</v>
       </c>
@@ -1069,7 +1068,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2035</v>
       </c>
@@ -1116,7 +1115,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2036</v>
       </c>
@@ -1163,7 +1162,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2037</v>
       </c>
@@ -1210,7 +1209,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2038</v>
       </c>
@@ -1257,7 +1256,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2039</v>
       </c>
@@ -1304,7 +1303,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2040</v>
       </c>
@@ -1351,7 +1350,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2041</v>
       </c>
@@ -1398,7 +1397,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2042</v>
       </c>
@@ -1445,7 +1444,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2043</v>
       </c>
@@ -1492,7 +1491,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2044</v>
       </c>
@@ -1539,7 +1538,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2045</v>
       </c>
@@ -1586,7 +1585,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2046</v>
       </c>
@@ -1633,7 +1632,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2047</v>
       </c>
@@ -1680,7 +1679,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2048</v>
       </c>
@@ -1727,7 +1726,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2049</v>
       </c>
@@ -1774,7 +1773,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2050</v>
       </c>

</xml_diff>

<commit_message>
add six-week O&M window and separate cable lay vessels
</commit_message>
<xml_diff>
--- a/analysis/library/investments/scenario-investments.xlsx
+++ b/analysis/library/investments/scenario-investments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhemez/Floating-CORAL/CORAL/analysis/library/investments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CEB459-4587-E44C-8C70-2018257CD1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28266BD-5570-2647-B60B-9B4F39716FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1420" windowWidth="28080" windowHeight="18500" activeTab="2" xr2:uid="{D6119032-A265-B843-9C0C-F79837C83C57}"/>
+    <workbookView xWindow="1440" yWindow="1780" windowWidth="28080" windowHeight="18500" xr2:uid="{D6119032-A265-B843-9C0C-F79837C83C57}"/>
   </bookViews>
   <sheets>
     <sheet name="Port-investments" sheetId="1" r:id="rId1"/>
@@ -587,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C454546C-8D82-6242-878C-E8FCE0FC7184}">
   <dimension ref="B2:P24"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -900,14 +900,14 @@
         <v>255</v>
       </c>
       <c r="N11" s="2">
-        <v>476</v>
+        <v>567</v>
       </c>
       <c r="O11" s="2">
-        <f t="shared" si="1"/>
-        <v>1171</v>
+        <f>K11+N11</f>
+        <v>1262</v>
       </c>
       <c r="P11" s="2">
-        <f t="shared" si="2"/>
+        <f>K11</f>
         <v>695</v>
       </c>
     </row>
@@ -1435,11 +1435,11 @@
       </c>
       <c r="M8">
         <f>'Port-investments'!P8+'Port-investments'!O11+'Port-investments'!P11</f>
-        <v>2579</v>
+        <v>2670</v>
       </c>
       <c r="N8">
         <f t="shared" si="4"/>
-        <v>7980</v>
+        <v>8071</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -1489,7 +1489,7 @@
       </c>
       <c r="N9">
         <f t="shared" si="4"/>
-        <v>7980</v>
+        <v>8071</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="N10">
         <f t="shared" si="4"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -1593,7 +1593,7 @@
       </c>
       <c r="N11">
         <f t="shared" si="4"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -1643,7 +1643,7 @@
       </c>
       <c r="N12">
         <f t="shared" si="4"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="N13">
         <f t="shared" si="4"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -1743,7 +1743,7 @@
       </c>
       <c r="N14">
         <f t="shared" si="4"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -1793,7 +1793,7 @@
       </c>
       <c r="N15">
         <f t="shared" si="4"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -1843,7 +1843,7 @@
       </c>
       <c r="N16">
         <f t="shared" si="4"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -1893,7 +1893,7 @@
       </c>
       <c r="N17">
         <f t="shared" si="4"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -1943,7 +1943,7 @@
       </c>
       <c r="N18">
         <f t="shared" si="4"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -2003,8 +2003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D2FA58B-1537-1640-9045-FA14C00D59E7}">
   <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView topLeftCell="M1" zoomScale="142" workbookViewId="0">
+      <selection activeCell="S37" sqref="S37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2199,7 +2199,7 @@
         <v>1274</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K36" si="2">J3/1000</f>
+        <f t="shared" ref="K3:K35" si="2">J3/1000</f>
         <v>1.274</v>
       </c>
       <c r="L3">
@@ -2464,7 +2464,7 @@
         <v>3451</v>
       </c>
       <c r="S6">
-        <f t="shared" si="10"/>
+        <f>S5+R6</f>
         <v>5401</v>
       </c>
       <c r="T6">
@@ -2685,15 +2685,15 @@
       </c>
       <c r="R9">
         <f>'Port-investments'!P8+'Port-investments'!O11+'Port-investments'!P11</f>
-        <v>2579</v>
+        <v>2670</v>
       </c>
       <c r="S9">
-        <f t="shared" si="10"/>
-        <v>7980</v>
+        <f>S8+R9</f>
+        <v>8071</v>
       </c>
       <c r="T9">
         <f t="shared" si="5"/>
-        <v>7.98</v>
+        <v>8.0709999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
@@ -2763,11 +2763,11 @@
       </c>
       <c r="S10">
         <f t="shared" si="10"/>
-        <v>7980</v>
+        <v>8071</v>
       </c>
       <c r="T10">
         <f t="shared" si="5"/>
-        <v>7.98</v>
+        <v>8.0709999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
@@ -2838,12 +2838,12 @@
         <v>2800</v>
       </c>
       <c r="S11">
-        <f t="shared" si="10"/>
-        <v>10780</v>
+        <f>S10+R11</f>
+        <v>10871</v>
       </c>
       <c r="T11">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
@@ -2915,11 +2915,11 @@
       </c>
       <c r="S12">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T12">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
@@ -2989,11 +2989,11 @@
       </c>
       <c r="S13">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T13">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
@@ -3063,11 +3063,11 @@
       </c>
       <c r="S14">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T14">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
@@ -3137,11 +3137,11 @@
       </c>
       <c r="S15">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T15">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
@@ -3211,11 +3211,11 @@
       </c>
       <c r="S16">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T16">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
@@ -3285,11 +3285,11 @@
       </c>
       <c r="S17">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T17">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
@@ -3359,11 +3359,11 @@
       </c>
       <c r="S18">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T18">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
@@ -3433,11 +3433,11 @@
       </c>
       <c r="S19">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T19">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
@@ -3507,11 +3507,11 @@
       </c>
       <c r="S20">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T20">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
@@ -3581,11 +3581,11 @@
       </c>
       <c r="S21">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T21">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
@@ -3655,11 +3655,11 @@
       </c>
       <c r="S22">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T22">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
@@ -3729,11 +3729,11 @@
       </c>
       <c r="S23">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T23">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
@@ -3803,11 +3803,11 @@
       </c>
       <c r="S24">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T24">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
@@ -3878,11 +3878,11 @@
       </c>
       <c r="S25">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T25">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
@@ -3953,11 +3953,11 @@
       </c>
       <c r="S26">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T26">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
@@ -4028,11 +4028,11 @@
       </c>
       <c r="S27">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T27">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
@@ -4103,11 +4103,11 @@
       </c>
       <c r="S28">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T28">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
@@ -4178,11 +4178,11 @@
       </c>
       <c r="S29">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T29">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
@@ -4253,11 +4253,11 @@
       </c>
       <c r="S30">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T30">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
@@ -4328,11 +4328,11 @@
       </c>
       <c r="S31">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T31">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
@@ -4403,11 +4403,11 @@
       </c>
       <c r="S32">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T32">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
@@ -4478,11 +4478,11 @@
       </c>
       <c r="S33">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T33">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
@@ -4553,11 +4553,11 @@
       </c>
       <c r="S34">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T34">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
@@ -4628,11 +4628,11 @@
       </c>
       <c r="S35">
         <f t="shared" si="10"/>
-        <v>10780</v>
+        <v>10871</v>
       </c>
       <c r="T35">
         <f t="shared" si="5"/>
-        <v>10.78</v>
+        <v>10.871</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edit figures and update AHTS/tug ratio
</commit_message>
<xml_diff>
--- a/analysis/library/investments/scenario-investments.xlsx
+++ b/analysis/library/investments/scenario-investments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhemez/Floating-CORAL/CORAL/analysis/library/investments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28266BD-5570-2647-B60B-9B4F39716FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838C34D0-8B01-9649-B3FC-4D3B691424C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="1780" windowWidth="28080" windowHeight="18500" xr2:uid="{D6119032-A265-B843-9C0C-F79837C83C57}"/>
   </bookViews>
@@ -587,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C454546C-8D82-6242-878C-E8FCE0FC7184}">
   <dimension ref="B2:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -807,11 +807,11 @@
         <v>476</v>
       </c>
       <c r="O8" s="2">
-        <f t="shared" ref="O8:O11" si="1">K8+N8</f>
+        <f t="shared" ref="O8:O10" si="1">K8+N8</f>
         <v>1189</v>
       </c>
       <c r="P8" s="2">
-        <f t="shared" ref="P8:P11" si="2">K8</f>
+        <f t="shared" ref="P8:P10" si="2">K8</f>
         <v>713</v>
       </c>
     </row>

</xml_diff>

<commit_message>
align with ORBIT and reformat figures
</commit_message>
<xml_diff>
--- a/analysis/library/investments/scenario-investments.xlsx
+++ b/analysis/library/investments/scenario-investments.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhemez/Floating-CORAL/CORAL/analysis/library/investments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838C34D0-8B01-9649-B3FC-4D3B691424C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B2FF38-37D6-9E49-A9A8-4447444E7336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1780" windowWidth="28080" windowHeight="18500" xr2:uid="{D6119032-A265-B843-9C0C-F79837C83C57}"/>
+    <workbookView xWindow="1440" yWindow="1780" windowWidth="28080" windowHeight="18500" activeTab="2" xr2:uid="{D6119032-A265-B843-9C0C-F79837C83C57}"/>
   </bookViews>
   <sheets>
     <sheet name="Port-investments" sheetId="1" r:id="rId1"/>
     <sheet name="schedule-short" sheetId="7" r:id="rId2"/>
     <sheet name="schedule" sheetId="8" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -587,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C454546C-8D82-6242-878C-E8FCE0FC7184}">
   <dimension ref="B2:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="E1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -763,24 +763,24 @@
         <v>4</v>
       </c>
       <c r="K7" s="2">
-        <v>676</v>
+        <v>700</v>
       </c>
       <c r="L7" s="2">
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="M7" s="2">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="N7" s="2">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="O7" s="2">
         <f>K7+N7</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="P7" s="2">
         <f>K7</f>
-        <v>676</v>
+        <v>700</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.2">
@@ -798,17 +798,17 @@
         <v>713</v>
       </c>
       <c r="L8" s="2">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="M8" s="2">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="N8" s="2">
-        <v>476</v>
+        <v>500</v>
       </c>
       <c r="O8" s="2">
         <f t="shared" ref="O8:O10" si="1">K8+N8</f>
-        <v>1189</v>
+        <v>1213</v>
       </c>
       <c r="P8" s="2">
         <f t="shared" ref="P8:P10" si="2">K8</f>
@@ -830,17 +830,17 @@
         <v>2800</v>
       </c>
       <c r="L9" s="2">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="M9" s="2">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="N9" s="2">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="O9" s="2">
         <f t="shared" si="1"/>
-        <v>2800</v>
+        <v>3200</v>
       </c>
       <c r="P9" s="2">
         <f t="shared" si="2"/>
@@ -856,7 +856,7 @@
         <v>6</v>
       </c>
       <c r="K10" s="2">
-        <v>1114</v>
+        <v>1100</v>
       </c>
       <c r="L10" s="2">
         <v>0</v>
@@ -865,15 +865,15 @@
         <v>0</v>
       </c>
       <c r="N10" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O10" s="2">
         <f t="shared" si="1"/>
-        <v>1148</v>
+        <v>1135</v>
       </c>
       <c r="P10" s="2">
         <f t="shared" si="2"/>
-        <v>1114</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
@@ -891,24 +891,24 @@
         <v>8</v>
       </c>
       <c r="K11" s="2">
-        <v>695</v>
+        <v>665</v>
       </c>
       <c r="L11" s="2">
-        <v>113</v>
+        <v>0</v>
       </c>
       <c r="M11" s="2">
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="N11" s="2">
-        <v>567</v>
+        <v>0</v>
       </c>
       <c r="O11" s="2">
         <f>K11+N11</f>
-        <v>1262</v>
+        <v>665</v>
       </c>
       <c r="P11" s="2">
         <f>K11</f>
-        <v>695</v>
+        <v>665</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
@@ -1009,7 +1009,7 @@
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1082,51 +1082,51 @@
       </c>
       <c r="C2">
         <f>'Port-investments'!O7</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="D2">
         <f>C2</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="E2">
         <f>'Port-investments'!$O$7</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="F2">
         <f>E2</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="G2">
         <f>'Port-investments'!$O$7</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="H2">
         <f>G2</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="I2">
         <f>'Port-investments'!$O$7</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="J2">
         <f>I2</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="K2">
         <f>'Port-investments'!$O$7</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="L2">
         <f>K2</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="M2">
         <f>'Port-investments'!$O$7</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="N2">
         <f>M2</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -1138,51 +1138,51 @@
       </c>
       <c r="C3">
         <f>'Port-investments'!P7</f>
-        <v>676</v>
+        <v>700</v>
       </c>
       <c r="D3">
         <f>D2+C3</f>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E3">
         <f>'Port-investments'!$P$7</f>
-        <v>676</v>
+        <v>700</v>
       </c>
       <c r="F3">
         <f>F2+E3</f>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="G3">
         <f>'Port-investments'!$P$7</f>
-        <v>676</v>
+        <v>700</v>
       </c>
       <c r="H3">
         <f>H2+G3</f>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="I3">
         <f>'Port-investments'!$P$7</f>
-        <v>676</v>
+        <v>700</v>
       </c>
       <c r="J3">
         <f>J2+I3</f>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="K3">
         <f>'Port-investments'!$P$7</f>
-        <v>676</v>
+        <v>700</v>
       </c>
       <c r="L3">
         <f>L2+K3</f>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="M3">
         <f>'Port-investments'!$P$7</f>
-        <v>676</v>
+        <v>700</v>
       </c>
       <c r="N3">
         <f>N2+M3</f>
-        <v>1950</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -1197,44 +1197,44 @@
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D18" si="0">D3+C4</f>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
         <f>F3+E4</f>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H18" si="1">H3+G4</f>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="I4">
         <f>'Port-investments'!O8</f>
-        <v>1189</v>
+        <v>1213</v>
       </c>
       <c r="J4">
         <f t="shared" ref="J4:J18" si="2">J3+I4</f>
-        <v>3139</v>
+        <v>3213</v>
       </c>
       <c r="K4">
         <f>'Port-investments'!O8</f>
-        <v>1189</v>
+        <v>1213</v>
       </c>
       <c r="L4">
         <f t="shared" ref="L4:L18" si="3">L3+K4</f>
-        <v>3139</v>
+        <v>3213</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N18" si="4">N3+M4</f>
-        <v>1950</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -1249,45 +1249,45 @@
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E5">
         <f>'Port-investments'!O10</f>
-        <v>1148</v>
+        <v>1135</v>
       </c>
       <c r="F5">
         <f>F4+E5</f>
-        <v>3098</v>
+        <v>3135</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
         <f t="shared" si="2"/>
-        <v>3139</v>
+        <v>3213</v>
       </c>
       <c r="K5">
         <f>'Port-investments'!O10</f>
-        <v>1148</v>
+        <v>1135</v>
       </c>
       <c r="L5">
         <f t="shared" si="3"/>
-        <v>4287</v>
+        <v>4348</v>
       </c>
       <c r="M5">
         <f>'Port-investments'!O8+'Port-investments'!O10+'Port-investments'!P10</f>
-        <v>3451</v>
+        <v>3448</v>
       </c>
       <c r="N5">
         <f t="shared" si="4"/>
-        <v>5401</v>
+        <v>5448</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -1302,42 +1302,42 @@
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
         <f t="shared" ref="F6:F18" si="5">F5+E6</f>
-        <v>3098</v>
+        <v>3135</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
         <f t="shared" si="2"/>
-        <v>3139</v>
+        <v>3213</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
         <f t="shared" si="3"/>
-        <v>4287</v>
+        <v>4348</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
         <f t="shared" si="4"/>
-        <v>5401</v>
+        <v>5448</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1352,43 +1352,43 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E7">
         <f>'Port-investments'!P10</f>
-        <v>1114</v>
+        <v>1100</v>
       </c>
       <c r="F7">
         <f t="shared" si="5"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
         <f t="shared" si="2"/>
-        <v>3139</v>
+        <v>3213</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
         <f t="shared" si="3"/>
-        <v>4287</v>
+        <v>4348</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
         <f t="shared" si="4"/>
-        <v>5401</v>
+        <v>5448</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -1403,43 +1403,43 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
         <f t="shared" si="5"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
         <f t="shared" si="2"/>
-        <v>3139</v>
+        <v>3213</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
         <f t="shared" si="3"/>
-        <v>4287</v>
+        <v>4348</v>
       </c>
       <c r="M8">
         <f>'Port-investments'!P8+'Port-investments'!O11+'Port-investments'!P11</f>
-        <v>2670</v>
+        <v>2043</v>
       </c>
       <c r="N8">
         <f t="shared" si="4"/>
-        <v>8071</v>
+        <v>7491</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -1454,42 +1454,42 @@
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
         <f t="shared" si="5"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
         <f t="shared" si="2"/>
-        <v>3139</v>
+        <v>3213</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
         <f t="shared" si="3"/>
-        <v>4287</v>
+        <v>4348</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
         <f t="shared" si="4"/>
-        <v>8071</v>
+        <v>7491</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -1504,44 +1504,44 @@
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
         <f t="shared" si="5"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="G10">
         <f>'Port-investments'!O9</f>
-        <v>2800</v>
+        <v>3200</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
         <f t="shared" si="2"/>
-        <v>3139</v>
+        <v>3213</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
         <f t="shared" si="3"/>
-        <v>4287</v>
+        <v>4348</v>
       </c>
       <c r="M10">
         <f>'Port-investments'!O9</f>
-        <v>2800</v>
+        <v>3200</v>
       </c>
       <c r="N10">
         <f t="shared" si="4"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -1556,21 +1556,21 @@
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
         <f t="shared" si="5"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="I11">
         <f>'Port-investments'!P8</f>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="J11">
         <f t="shared" si="2"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="K11">
         <f>'Port-investments'!P8</f>
@@ -1586,14 +1586,14 @@
       </c>
       <c r="L11">
         <f t="shared" si="3"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11">
         <f t="shared" si="4"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -1608,42 +1608,42 @@
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
         <f t="shared" si="5"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
         <f t="shared" si="1"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12">
         <f t="shared" si="2"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
         <f t="shared" si="3"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
       <c r="N12">
         <f t="shared" si="4"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -1658,42 +1658,42 @@
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
         <f t="shared" si="5"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
         <f t="shared" si="1"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13">
         <f t="shared" si="2"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13">
         <f t="shared" si="3"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13">
         <f t="shared" si="4"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -1708,42 +1708,42 @@
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
         <f t="shared" si="5"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
         <f t="shared" si="1"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
       <c r="J14">
         <f t="shared" si="2"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
         <f t="shared" si="3"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14">
         <f t="shared" si="4"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -1758,42 +1758,42 @@
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
         <f t="shared" si="5"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
         <f t="shared" si="1"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15">
         <f t="shared" si="2"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
         <f t="shared" si="3"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15">
         <f t="shared" si="4"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -1808,42 +1808,42 @@
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
         <f t="shared" si="5"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
         <f t="shared" si="1"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16">
         <f t="shared" si="2"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
         <f t="shared" si="3"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16">
         <f t="shared" si="4"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -1858,42 +1858,42 @@
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
         <f t="shared" si="5"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
         <f t="shared" si="1"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="I17">
         <v>0</v>
       </c>
       <c r="J17">
         <f t="shared" si="2"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
         <f t="shared" si="3"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
       <c r="N17">
         <f t="shared" si="4"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -1908,42 +1908,42 @@
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
         <f t="shared" si="5"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
         <f t="shared" si="1"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
       <c r="J18">
         <f t="shared" si="2"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
         <f t="shared" si="3"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="M18">
         <v>0</v>
       </c>
       <c r="N18">
         <f t="shared" si="4"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -2003,8 +2003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D2FA58B-1537-1640-9045-FA14C00D59E7}">
   <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="S37" sqref="S37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="142" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2168,75 +2168,75 @@
       </c>
       <c r="C3">
         <f>'Port-investments'!O7</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="D3">
         <f>C3</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E35" si="0">D3/1000</f>
-        <v>1.274</v>
+        <f>D3/1000</f>
+        <v>1.3</v>
       </c>
       <c r="F3">
         <f>'Port-investments'!$O$7</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="G3">
         <f>F3</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H35" si="1">G3/1000</f>
-        <v>1.274</v>
+        <f t="shared" ref="H3:H35" si="0">G3/1000</f>
+        <v>1.3</v>
       </c>
       <c r="I3">
         <f>'Port-investments'!$O$7</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="J3">
         <f>I3</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K35" si="2">J3/1000</f>
-        <v>1.274</v>
+        <f t="shared" ref="K3:K35" si="1">J3/1000</f>
+        <v>1.3</v>
       </c>
       <c r="L3">
         <f>'Port-investments'!$O$7</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="M3">
         <f>L3</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N35" si="3">M3/1000</f>
-        <v>1.274</v>
+        <f t="shared" ref="N3:N35" si="2">M3/1000</f>
+        <v>1.3</v>
       </c>
       <c r="O3">
         <f>'Port-investments'!$O$7</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="P3">
         <f>O3</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q35" si="4">P3/1000</f>
-        <v>1.274</v>
+        <f t="shared" ref="Q3:Q35" si="3">P3/1000</f>
+        <v>1.3</v>
       </c>
       <c r="R3">
         <f>'Port-investments'!$O$7</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="S3">
         <f>R3</f>
-        <v>1274</v>
+        <v>1300</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T35" si="5">S3/1000</f>
-        <v>1.274</v>
+        <f t="shared" ref="T3:T35" si="4">S3/1000</f>
+        <v>1.3</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -2248,75 +2248,75 @@
       </c>
       <c r="C4">
         <f>'Port-investments'!P7</f>
-        <v>676</v>
+        <v>700</v>
       </c>
       <c r="D4">
         <f>D3+C4</f>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" ref="E4:E35" si="5">D4/1000</f>
+        <v>2</v>
       </c>
       <c r="F4">
         <f>'Port-investments'!$P$7</f>
-        <v>676</v>
+        <v>700</v>
       </c>
       <c r="G4">
         <f>G3+F4</f>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
-        <v>1.95</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="I4">
         <f>'Port-investments'!$P$7</f>
-        <v>676</v>
+        <v>700</v>
       </c>
       <c r="J4">
         <f>J3+I4</f>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="K4">
-        <f t="shared" si="2"/>
-        <v>1.95</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="L4">
         <f>'Port-investments'!$P$7</f>
-        <v>676</v>
+        <v>700</v>
       </c>
       <c r="M4">
         <f>M3+L4</f>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="N4">
-        <f t="shared" si="3"/>
-        <v>1.95</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="O4">
         <f>'Port-investments'!$P$7</f>
-        <v>676</v>
+        <v>700</v>
       </c>
       <c r="P4">
         <f>P3+O4</f>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="4"/>
-        <v>1.95</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="R4">
         <f>'Port-investments'!$P$7</f>
-        <v>676</v>
+        <v>700</v>
       </c>
       <c r="S4">
         <f>S3+R4</f>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="T4">
-        <f t="shared" si="5"/>
-        <v>1.95</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
@@ -2331,68 +2331,68 @@
       </c>
       <c r="D5">
         <f t="shared" ref="D5:D35" si="6">D4+C5</f>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
         <f>G4+F5</f>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
-        <v>1.95</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
         <f t="shared" ref="J5:J35" si="7">J4+I5</f>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="K5">
-        <f t="shared" si="2"/>
-        <v>1.95</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="L5">
         <f>'Port-investments'!O8</f>
-        <v>1189</v>
+        <v>1213</v>
       </c>
       <c r="M5">
         <f t="shared" ref="M5:M35" si="8">M4+L5</f>
-        <v>3139</v>
+        <v>3213</v>
       </c>
       <c r="N5">
-        <f t="shared" si="3"/>
-        <v>3.1389999999999998</v>
+        <f t="shared" si="2"/>
+        <v>3.2130000000000001</v>
       </c>
       <c r="O5">
         <f>'Port-investments'!O8</f>
-        <v>1189</v>
+        <v>1213</v>
       </c>
       <c r="P5">
         <f t="shared" ref="P5:P35" si="9">P4+O5</f>
-        <v>3139</v>
+        <v>3213</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="4"/>
-        <v>3.1389999999999998</v>
+        <f t="shared" si="3"/>
+        <v>3.2130000000000001</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
       <c r="S5">
         <f t="shared" ref="S5:S35" si="10">S4+R5</f>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="T5">
-        <f t="shared" si="5"/>
-        <v>1.95</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
@@ -2407,69 +2407,69 @@
       </c>
       <c r="D6">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F6">
         <f>'Port-investments'!O10</f>
-        <v>1148</v>
+        <v>1135</v>
       </c>
       <c r="G6">
         <f>G5+F6</f>
-        <v>3098</v>
+        <v>3135</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
-        <v>3.0979999999999999</v>
+        <f t="shared" si="0"/>
+        <v>3.1349999999999998</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
         <f t="shared" si="7"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="K6">
-        <f t="shared" si="2"/>
-        <v>1.95</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
         <f t="shared" si="8"/>
-        <v>3139</v>
+        <v>3213</v>
       </c>
       <c r="N6">
-        <f t="shared" si="3"/>
-        <v>3.1389999999999998</v>
+        <f t="shared" si="2"/>
+        <v>3.2130000000000001</v>
       </c>
       <c r="O6">
         <f>'Port-investments'!O10</f>
-        <v>1148</v>
+        <v>1135</v>
       </c>
       <c r="P6">
         <f t="shared" si="9"/>
-        <v>4287</v>
+        <v>4348</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="4"/>
-        <v>4.2869999999999999</v>
+        <f t="shared" si="3"/>
+        <v>4.3479999999999999</v>
       </c>
       <c r="R6">
         <f>'Port-investments'!O8+'Port-investments'!O10+'Port-investments'!P10</f>
-        <v>3451</v>
+        <v>3448</v>
       </c>
       <c r="S6">
         <f>S5+R6</f>
-        <v>5401</v>
+        <v>5448</v>
       </c>
       <c r="T6">
-        <f t="shared" si="5"/>
-        <v>5.4009999999999998</v>
+        <f t="shared" si="4"/>
+        <v>5.4480000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
@@ -2484,66 +2484,66 @@
       </c>
       <c r="D7">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
         <f t="shared" ref="G7:G35" si="11">G6+F7</f>
-        <v>3098</v>
+        <v>3135</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
-        <v>3.0979999999999999</v>
+        <f t="shared" si="0"/>
+        <v>3.1349999999999998</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
         <f t="shared" si="7"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="K7">
-        <f t="shared" si="2"/>
-        <v>1.95</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
         <f t="shared" si="8"/>
-        <v>3139</v>
+        <v>3213</v>
       </c>
       <c r="N7">
-        <f t="shared" si="3"/>
-        <v>3.1389999999999998</v>
+        <f t="shared" si="2"/>
+        <v>3.2130000000000001</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7">
         <f t="shared" si="9"/>
-        <v>4287</v>
+        <v>4348</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="4"/>
-        <v>4.2869999999999999</v>
+        <f t="shared" si="3"/>
+        <v>4.3479999999999999</v>
       </c>
       <c r="R7">
         <v>0</v>
       </c>
       <c r="S7">
         <f t="shared" si="10"/>
-        <v>5401</v>
+        <v>5448</v>
       </c>
       <c r="T7">
-        <f t="shared" si="5"/>
-        <v>5.4009999999999998</v>
+        <f t="shared" si="4"/>
+        <v>5.4480000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
@@ -2558,67 +2558,67 @@
       </c>
       <c r="D8">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F8">
         <f>'Port-investments'!P10</f>
-        <v>1114</v>
+        <v>1100</v>
       </c>
       <c r="G8">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
         <f t="shared" si="7"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="K8">
-        <f t="shared" si="2"/>
-        <v>1.95</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
         <f t="shared" si="8"/>
-        <v>3139</v>
+        <v>3213</v>
       </c>
       <c r="N8">
-        <f t="shared" si="3"/>
-        <v>3.1389999999999998</v>
+        <f t="shared" si="2"/>
+        <v>3.2130000000000001</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8">
         <f t="shared" si="9"/>
-        <v>4287</v>
+        <v>4348</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="4"/>
-        <v>4.2869999999999999</v>
+        <f t="shared" si="3"/>
+        <v>4.3479999999999999</v>
       </c>
       <c r="R8">
         <v>0</v>
       </c>
       <c r="S8">
         <f t="shared" si="10"/>
-        <v>5401</v>
+        <v>5448</v>
       </c>
       <c r="T8">
-        <f t="shared" si="5"/>
-        <v>5.4009999999999998</v>
+        <f t="shared" si="4"/>
+        <v>5.4480000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
@@ -2633,67 +2633,67 @@
       </c>
       <c r="D9">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
         <f t="shared" si="7"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="K9">
-        <f t="shared" si="2"/>
-        <v>1.95</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
         <f t="shared" si="8"/>
-        <v>3139</v>
+        <v>3213</v>
       </c>
       <c r="N9">
-        <f t="shared" si="3"/>
-        <v>3.1389999999999998</v>
+        <f t="shared" si="2"/>
+        <v>3.2130000000000001</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9">
         <f t="shared" si="9"/>
-        <v>4287</v>
+        <v>4348</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="4"/>
-        <v>4.2869999999999999</v>
+        <f t="shared" si="3"/>
+        <v>4.3479999999999999</v>
       </c>
       <c r="R9">
         <f>'Port-investments'!P8+'Port-investments'!O11+'Port-investments'!P11</f>
-        <v>2670</v>
+        <v>2043</v>
       </c>
       <c r="S9">
         <f>S8+R9</f>
-        <v>8071</v>
+        <v>7491</v>
       </c>
       <c r="T9">
-        <f t="shared" si="5"/>
-        <v>8.0709999999999997</v>
+        <f t="shared" si="4"/>
+        <v>7.4909999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
@@ -2708,66 +2708,66 @@
       </c>
       <c r="D10">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
         <f t="shared" si="7"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="K10">
-        <f t="shared" si="2"/>
-        <v>1.95</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
         <f t="shared" si="8"/>
-        <v>3139</v>
+        <v>3213</v>
       </c>
       <c r="N10">
-        <f t="shared" si="3"/>
-        <v>3.1389999999999998</v>
+        <f t="shared" si="2"/>
+        <v>3.2130000000000001</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10">
         <f t="shared" si="9"/>
-        <v>4287</v>
+        <v>4348</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="4"/>
-        <v>4.2869999999999999</v>
+        <f t="shared" si="3"/>
+        <v>4.3479999999999999</v>
       </c>
       <c r="R10">
         <v>0</v>
       </c>
       <c r="S10">
         <f t="shared" si="10"/>
-        <v>8071</v>
+        <v>7491</v>
       </c>
       <c r="T10">
-        <f t="shared" si="5"/>
-        <v>8.0709999999999997</v>
+        <f t="shared" si="4"/>
+        <v>7.4909999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
@@ -2782,68 +2782,68 @@
       </c>
       <c r="D11">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I11">
         <f>'Port-investments'!O9</f>
-        <v>2800</v>
+        <v>3200</v>
       </c>
       <c r="J11">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K11">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
         <f t="shared" si="8"/>
-        <v>3139</v>
+        <v>3213</v>
       </c>
       <c r="N11">
-        <f t="shared" si="3"/>
-        <v>3.1389999999999998</v>
+        <f t="shared" si="2"/>
+        <v>3.2130000000000001</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11">
         <f t="shared" si="9"/>
-        <v>4287</v>
+        <v>4348</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="4"/>
-        <v>4.2869999999999999</v>
+        <f t="shared" si="3"/>
+        <v>4.3479999999999999</v>
       </c>
       <c r="R11">
         <f>'Port-investments'!O9</f>
-        <v>2800</v>
+        <v>3200</v>
       </c>
       <c r="S11">
         <f>S10+R11</f>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T11">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
@@ -2858,33 +2858,33 @@
       </c>
       <c r="D12">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H12">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K12">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L12">
         <f>'Port-investments'!P8</f>
@@ -2892,11 +2892,11 @@
       </c>
       <c r="M12">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N12">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O12">
         <f>'Port-investments'!P8</f>
@@ -2904,22 +2904,22 @@
       </c>
       <c r="P12">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R12">
         <v>0</v>
       </c>
       <c r="S12">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T12">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
@@ -2934,66 +2934,66 @@
       </c>
       <c r="D13">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K13">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N13">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R13">
         <v>0</v>
       </c>
       <c r="S13">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T13">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
@@ -3008,66 +3008,66 @@
       </c>
       <c r="D14">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H14">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
       <c r="J14">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K14">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N14">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R14">
         <v>0</v>
       </c>
       <c r="S14">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T14">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
@@ -3082,66 +3082,66 @@
       </c>
       <c r="D15">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H15">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K15">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N15">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R15">
         <v>0</v>
       </c>
       <c r="S15">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T15">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
@@ -3156,66 +3156,66 @@
       </c>
       <c r="D16">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H16">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K16">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N16">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R16">
         <v>0</v>
       </c>
       <c r="S16">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T16">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
@@ -3230,66 +3230,66 @@
       </c>
       <c r="D17">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H17">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I17">
         <v>0</v>
       </c>
       <c r="J17">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K17">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N17">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
       <c r="P17">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R17">
         <v>0</v>
       </c>
       <c r="S17">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T17">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
@@ -3304,66 +3304,66 @@
       </c>
       <c r="D18">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H18">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
       <c r="J18">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K18">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N18">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O18">
         <v>0</v>
       </c>
       <c r="P18">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R18">
         <v>0</v>
       </c>
       <c r="S18">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T18">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
@@ -3378,66 +3378,66 @@
       </c>
       <c r="D19">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H19">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I19">
         <v>0</v>
       </c>
       <c r="J19">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K19">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N19">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O19">
         <v>0</v>
       </c>
       <c r="P19">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R19">
         <v>0</v>
       </c>
       <c r="S19">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T19">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
@@ -3452,66 +3452,66 @@
       </c>
       <c r="D20">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H20">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I20">
         <v>0</v>
       </c>
       <c r="J20">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K20">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N20">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O20">
         <v>0</v>
       </c>
       <c r="P20">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R20">
         <v>0</v>
       </c>
       <c r="S20">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T20">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
@@ -3526,66 +3526,66 @@
       </c>
       <c r="D21">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="G21">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H21">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I21">
         <v>0</v>
       </c>
       <c r="J21">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K21">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N21">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O21">
         <v>0</v>
       </c>
       <c r="P21">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R21">
         <v>0</v>
       </c>
       <c r="S21">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T21">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
@@ -3600,66 +3600,66 @@
       </c>
       <c r="D22">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
       <c r="G22">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H22">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I22">
         <v>0</v>
       </c>
       <c r="J22">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K22">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L22">
         <v>0</v>
       </c>
       <c r="M22">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N22">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O22">
         <v>0</v>
       </c>
       <c r="P22">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R22">
         <v>0</v>
       </c>
       <c r="S22">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T22">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
@@ -3674,66 +3674,66 @@
       </c>
       <c r="D23">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
       <c r="G23">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H23">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I23">
         <v>0</v>
       </c>
       <c r="J23">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K23">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L23">
         <v>0</v>
       </c>
       <c r="M23">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N23">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O23">
         <v>0</v>
       </c>
       <c r="P23">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R23">
         <v>0</v>
       </c>
       <c r="S23">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T23">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
@@ -3748,66 +3748,66 @@
       </c>
       <c r="D24">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F24">
         <v>0</v>
       </c>
       <c r="G24">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H24">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I24">
         <v>0</v>
       </c>
       <c r="J24">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K24">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L24">
         <v>0</v>
       </c>
       <c r="M24">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N24">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O24">
         <v>0</v>
       </c>
       <c r="P24">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R24">
         <v>0</v>
       </c>
       <c r="S24">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T24">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
@@ -3823,66 +3823,66 @@
       </c>
       <c r="D25">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
       <c r="G25">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H25">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I25">
         <v>0</v>
       </c>
       <c r="J25">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K25">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
       <c r="M25">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N25">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O25">
         <v>0</v>
       </c>
       <c r="P25">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R25">
         <v>0</v>
       </c>
       <c r="S25">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T25">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
@@ -3898,66 +3898,66 @@
       </c>
       <c r="D26">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E26">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
       <c r="G26">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H26">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I26">
         <v>0</v>
       </c>
       <c r="J26">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K26">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L26">
         <v>0</v>
       </c>
       <c r="M26">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N26">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O26">
         <v>0</v>
       </c>
       <c r="P26">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R26">
         <v>0</v>
       </c>
       <c r="S26">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T26">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
@@ -3973,66 +3973,66 @@
       </c>
       <c r="D27">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E27">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F27">
         <v>0</v>
       </c>
       <c r="G27">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H27">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I27">
         <v>0</v>
       </c>
       <c r="J27">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K27">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L27">
         <v>0</v>
       </c>
       <c r="M27">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N27">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O27">
         <v>0</v>
       </c>
       <c r="P27">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R27">
         <v>0</v>
       </c>
       <c r="S27">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T27">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
@@ -4048,66 +4048,66 @@
       </c>
       <c r="D28">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F28">
         <v>0</v>
       </c>
       <c r="G28">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H28">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I28">
         <v>0</v>
       </c>
       <c r="J28">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K28">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L28">
         <v>0</v>
       </c>
       <c r="M28">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N28">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O28">
         <v>0</v>
       </c>
       <c r="P28">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R28">
         <v>0</v>
       </c>
       <c r="S28">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T28">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
@@ -4123,66 +4123,66 @@
       </c>
       <c r="D29">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
       <c r="G29">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H29">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I29">
         <v>0</v>
       </c>
       <c r="J29">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K29">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L29">
         <v>0</v>
       </c>
       <c r="M29">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N29">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O29">
         <v>0</v>
       </c>
       <c r="P29">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R29">
         <v>0</v>
       </c>
       <c r="S29">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T29">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
@@ -4198,66 +4198,66 @@
       </c>
       <c r="D30">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
       <c r="G30">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H30">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I30">
         <v>0</v>
       </c>
       <c r="J30">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K30">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L30">
         <v>0</v>
       </c>
       <c r="M30">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N30">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O30">
         <v>0</v>
       </c>
       <c r="P30">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R30">
         <v>0</v>
       </c>
       <c r="S30">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T30">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
@@ -4273,66 +4273,66 @@
       </c>
       <c r="D31">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F31">
         <v>0</v>
       </c>
       <c r="G31">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H31">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I31">
         <v>0</v>
       </c>
       <c r="J31">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K31">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L31">
         <v>0</v>
       </c>
       <c r="M31">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N31">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O31">
         <v>0</v>
       </c>
       <c r="P31">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R31">
         <v>0</v>
       </c>
       <c r="S31">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T31">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
@@ -4348,66 +4348,66 @@
       </c>
       <c r="D32">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E32">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F32">
         <v>0</v>
       </c>
       <c r="G32">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H32">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I32">
         <v>0</v>
       </c>
       <c r="J32">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K32">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L32">
         <v>0</v>
       </c>
       <c r="M32">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N32">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O32">
         <v>0</v>
       </c>
       <c r="P32">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R32">
         <v>0</v>
       </c>
       <c r="S32">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T32">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
@@ -4423,66 +4423,66 @@
       </c>
       <c r="D33">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F33">
         <v>0</v>
       </c>
       <c r="G33">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H33">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I33">
         <v>0</v>
       </c>
       <c r="J33">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K33">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L33">
         <v>0</v>
       </c>
       <c r="M33">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N33">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O33">
         <v>0</v>
       </c>
       <c r="P33">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R33">
         <v>0</v>
       </c>
       <c r="S33">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T33">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
@@ -4498,66 +4498,66 @@
       </c>
       <c r="D34">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F34">
         <v>0</v>
       </c>
       <c r="G34">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H34">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I34">
         <v>0</v>
       </c>
       <c r="J34">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K34">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L34">
         <v>0</v>
       </c>
       <c r="M34">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N34">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O34">
         <v>0</v>
       </c>
       <c r="P34">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R34">
         <v>0</v>
       </c>
       <c r="S34">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T34">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
@@ -4573,66 +4573,66 @@
       </c>
       <c r="D35">
         <f t="shared" si="6"/>
-        <v>1950</v>
+        <v>2000</v>
       </c>
       <c r="E35">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
       <c r="G35">
         <f t="shared" si="11"/>
-        <v>4212</v>
+        <v>4235</v>
       </c>
       <c r="H35">
-        <f t="shared" si="1"/>
-        <v>4.2119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>4.2350000000000003</v>
       </c>
       <c r="I35">
         <v>0</v>
       </c>
       <c r="J35">
         <f t="shared" si="7"/>
-        <v>4750</v>
+        <v>5200</v>
       </c>
       <c r="K35">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
+        <f t="shared" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="L35">
         <v>0</v>
       </c>
       <c r="M35">
         <f t="shared" si="8"/>
-        <v>3852</v>
+        <v>3926</v>
       </c>
       <c r="N35">
-        <f t="shared" si="3"/>
-        <v>3.8519999999999999</v>
+        <f t="shared" si="2"/>
+        <v>3.9260000000000002</v>
       </c>
       <c r="O35">
         <v>0</v>
       </c>
       <c r="P35">
         <f t="shared" si="9"/>
-        <v>5000</v>
+        <v>5061</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>5.0609999999999999</v>
       </c>
       <c r="R35">
         <v>0</v>
       </c>
       <c r="S35">
         <f t="shared" si="10"/>
-        <v>10871</v>
+        <v>10691</v>
       </c>
       <c r="T35">
-        <f t="shared" si="5"/>
-        <v>10.871</v>
+        <f t="shared" si="4"/>
+        <v>10.691000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial update to naming conventions (25 GW-high)'
</commit_message>
<xml_diff>
--- a/analysis/library/investments/scenario-investments.xlsx
+++ b/analysis/library/investments/scenario-investments.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhemez/Floating-CORAL/CORAL/analysis/library/investments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\West Coast ports\Analysis\Deployment\CORAL\analysis\library\investments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B2FF38-37D6-9E49-A9A8-4447444E7336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56558710-0E60-465B-9D30-9BCF7745EF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1780" windowWidth="28080" windowHeight="18500" activeTab="2" xr2:uid="{D6119032-A265-B843-9C0C-F79837C83C57}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{D6119032-A265-B843-9C0C-F79837C83C57}"/>
   </bookViews>
   <sheets>
     <sheet name="Port-investments" sheetId="1" r:id="rId1"/>
     <sheet name="schedule-short" sheetId="7" r:id="rId2"/>
     <sheet name="schedule" sheetId="8" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t>Port</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>Baseline-Low-million</t>
+  </si>
+  <si>
+    <t>25 GW - High (SC)</t>
   </si>
 </sst>
 </file>
@@ -591,7 +594,7 @@
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.5" customWidth="1"/>
@@ -609,7 +612,7 @@
     <col min="15" max="16" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -635,7 +638,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>2029</v>
       </c>
@@ -670,7 +673,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B4">
         <f t="shared" ref="B4:B24" si="0">B3+1</f>
         <v>2030</v>
@@ -706,7 +709,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B5">
         <f t="shared" si="0"/>
         <v>2031</v>
@@ -718,7 +721,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B6">
         <f t="shared" si="0"/>
         <v>2032</v>
@@ -754,7 +757,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B7">
         <f t="shared" si="0"/>
         <v>2033</v>
@@ -783,7 +786,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B8">
         <f t="shared" si="0"/>
         <v>2034</v>
@@ -815,7 +818,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B9">
         <f t="shared" si="0"/>
         <v>2035</v>
@@ -847,7 +850,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B10">
         <f t="shared" si="0"/>
         <v>2036</v>
@@ -876,7 +879,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B11">
         <f t="shared" si="0"/>
         <v>2037</v>
@@ -911,7 +914,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B12">
         <f t="shared" si="0"/>
         <v>2038</v>
@@ -923,73 +926,73 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B13">
         <f t="shared" si="0"/>
         <v>2039</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B14">
         <f t="shared" si="0"/>
         <v>2040</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B15">
         <f t="shared" si="0"/>
         <v>2041</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B16">
         <f t="shared" si="0"/>
         <v>2042</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17">
         <f t="shared" si="0"/>
         <v>2043</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18">
         <f t="shared" si="0"/>
         <v>2044</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19">
         <f t="shared" si="0"/>
         <v>2045</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20">
         <f t="shared" si="0"/>
         <v>2046</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21">
         <f t="shared" si="0"/>
         <v>2047</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B22">
         <f t="shared" si="0"/>
         <v>2048</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B23">
         <f t="shared" si="0"/>
         <v>2049</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B24">
         <f t="shared" si="0"/>
         <v>2050</v>
@@ -1012,7 +1015,7 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
@@ -1029,7 +1032,7 @@
     <col min="14" max="14" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1073,7 +1076,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2029</v>
       </c>
@@ -1129,7 +1132,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2030</v>
       </c>
@@ -1185,7 +1188,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2031</v>
       </c>
@@ -1237,7 +1240,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2032</v>
       </c>
@@ -1290,7 +1293,7 @@
         <v>5448</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2033</v>
       </c>
@@ -1340,7 +1343,7 @@
         <v>5448</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2034</v>
       </c>
@@ -1391,7 +1394,7 @@
         <v>5448</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2035</v>
       </c>
@@ -1442,7 +1445,7 @@
         <v>7491</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2036</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>7491</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2037</v>
       </c>
@@ -1544,7 +1547,7 @@
         <v>10691</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2038</v>
       </c>
@@ -1596,7 +1599,7 @@
         <v>10691</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2039</v>
       </c>
@@ -1646,7 +1649,7 @@
         <v>10691</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2040</v>
       </c>
@@ -1696,7 +1699,7 @@
         <v>10691</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2041</v>
       </c>
@@ -1746,7 +1749,7 @@
         <v>10691</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2042</v>
       </c>
@@ -1796,7 +1799,7 @@
         <v>10691</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2043</v>
       </c>
@@ -1846,7 +1849,7 @@
         <v>10691</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2044</v>
       </c>
@@ -1896,7 +1899,7 @@
         <v>10691</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2045</v>
       </c>
@@ -1946,52 +1949,52 @@
         <v>10691</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B25" s="4"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B27" s="4"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="4"/>
     </row>
   </sheetData>
@@ -2003,11 +2006,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D2FA58B-1537-1640-9045-FA14C00D59E7}">
   <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="142" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
@@ -2029,7 +2032,7 @@
     <col min="19" max="19" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2052,7 +2055,7 @@
         <v>52</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="I1" t="s">
         <v>14</v>
@@ -2091,7 +2094,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2028</v>
       </c>
@@ -2159,7 +2162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2029</v>
       </c>
@@ -2239,7 +2242,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2030</v>
       </c>
@@ -2319,7 +2322,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2031</v>
       </c>
@@ -2395,7 +2398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2032</v>
       </c>
@@ -2472,7 +2475,7 @@
         <v>5.4480000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2033</v>
       </c>
@@ -2546,7 +2549,7 @@
         <v>5.4480000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2034</v>
       </c>
@@ -2621,7 +2624,7 @@
         <v>5.4480000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2035</v>
       </c>
@@ -2696,7 +2699,7 @@
         <v>7.4909999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2036</v>
       </c>
@@ -2770,7 +2773,7 @@
         <v>7.4909999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2037</v>
       </c>
@@ -2846,7 +2849,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2038</v>
       </c>
@@ -2922,7 +2925,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2039</v>
       </c>
@@ -2996,7 +2999,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2040</v>
       </c>
@@ -3070,7 +3073,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2041</v>
       </c>
@@ -3144,7 +3147,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2042</v>
       </c>
@@ -3218,7 +3221,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2043</v>
       </c>
@@ -3292,7 +3295,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2044</v>
       </c>
@@ -3366,7 +3369,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2045</v>
       </c>
@@ -3440,7 +3443,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2046</v>
       </c>
@@ -3514,7 +3517,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2047</v>
       </c>
@@ -3588,7 +3591,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2048</v>
       </c>
@@ -3662,7 +3665,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2049</v>
       </c>
@@ -3736,7 +3739,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2050</v>
       </c>
@@ -3810,7 +3813,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25">
         <f>A24+1</f>
         <v>2051</v>
@@ -3885,7 +3888,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" ref="A26:A35" si="12">A25+1</f>
         <v>2052</v>
@@ -3960,7 +3963,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="12"/>
         <v>2053</v>
@@ -4035,7 +4038,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28">
         <f t="shared" si="12"/>
         <v>2054</v>
@@ -4110,7 +4113,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29">
         <f t="shared" si="12"/>
         <v>2055</v>
@@ -4185,7 +4188,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30">
         <f t="shared" si="12"/>
         <v>2056</v>
@@ -4260,7 +4263,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31">
         <f t="shared" si="12"/>
         <v>2057</v>
@@ -4335,7 +4338,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32">
         <f t="shared" si="12"/>
         <v>2058</v>
@@ -4410,7 +4413,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="12"/>
         <v>2059</v>
@@ -4485,7 +4488,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A34">
         <f t="shared" si="12"/>
         <v>2060</v>
@@ -4560,7 +4563,7 @@
         <v>10.691000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A35">
         <f t="shared" si="12"/>
         <v>2061</v>

</xml_diff>

<commit_message>
Update CORAL gantt charts per scenario
</commit_message>
<xml_diff>
--- a/analysis/library/investments/scenario-investments.xlsx
+++ b/analysis/library/investments/scenario-investments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\West Coast ports\Analysis\Deployment\CORAL\analysis\library\investments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DD48B0-74F4-49A3-8973-40063B5089E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5AD5659-A312-4A24-8103-4A4BF12C6D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{D6119032-A265-B843-9C0C-F79837C83C57}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" activeTab="2" xr2:uid="{D6119032-A265-B843-9C0C-F79837C83C57}"/>
   </bookViews>
   <sheets>
     <sheet name="Port-investments" sheetId="1" r:id="rId1"/>
@@ -202,19 +202,19 @@
     <t>Baseline-Low-million</t>
   </si>
   <si>
-    <t>25 GW - High (SC)</t>
-  </si>
-  <si>
-    <t>25 GW - Low</t>
-  </si>
-  <si>
-    <t>25 GW - High (CC)</t>
-  </si>
-  <si>
     <t>35 GW</t>
   </si>
   <si>
     <t>55 GW</t>
+  </si>
+  <si>
+    <t>25 GW</t>
+  </si>
+  <si>
+    <t>25 GW (SC)</t>
+  </si>
+  <si>
+    <t>25 GW (CC)</t>
   </si>
 </sst>
 </file>
@@ -602,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C454546C-8D82-6242-878C-E8FCE0FC7184}">
   <dimension ref="B2:P24"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2018,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D2FA58B-1537-1640-9045-FA14C00D59E7}">
   <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2058,7 +2058,7 @@
         <v>53</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F1" t="s">
         <v>12</v>
@@ -2067,7 +2067,7 @@
         <v>52</v>
       </c>
       <c r="H1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="I1" t="s">
         <v>14</v>
@@ -2076,7 +2076,7 @@
         <v>51</v>
       </c>
       <c r="K1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="L1" t="s">
         <v>16</v>
@@ -2094,7 +2094,7 @@
         <v>49</v>
       </c>
       <c r="Q1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="R1" t="s">
         <v>20</v>
@@ -2103,7 +2103,7 @@
         <v>48</v>
       </c>
       <c r="T1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">

</xml_diff>